<commit_message>
Repared bug with XMLS report calculations, optimmized XMLS report appearance.
</commit_message>
<xml_diff>
--- a/Reports/FinancialReportByVendor.xlsx
+++ b/Reports/FinancialReportByVendor.xlsx
@@ -55,9 +55,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000" tint="0"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -80,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -88,16 +94,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0">
       <alignment vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -135,123 +149,130 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2" s="2">
         <v>548.25</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2" s="2">
         <v>55</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2" s="2">
         <v>65.789999999999992</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>427.46000000000004</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="2">
         <v>77</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="2">
         <v>35</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3" s="2">
         <v>179.6188</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>-137.6188</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4" s="2">
         <v>555</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4" s="2">
         <v>25</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4" s="2">
         <v>168.834</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>361.166</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5" s="2">
         <v>184.5</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5" s="2">
         <v>15</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5" s="2">
         <v>167.115</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>2.3849999999999909</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6" s="2">
         <v>482.99999999999994</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6" s="2">
         <v>55</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6" s="2">
         <v>60.99499999999999</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>367.00499999999994</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7" s="2">
         <v>482.85</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7" s="2">
         <v>66</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7" s="2">
         <v>187.5285</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>229.32150000000002</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8" s="2">
         <v>246.5</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8" s="2">
         <v>45</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8" s="2">
         <v>27.115</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>174.385</v>
       </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <headerFooter/>

</xml_diff>